<commit_message>
adding support for 2 more reports
</commit_message>
<xml_diff>
--- a/src/ChurchBudgetReportGenerator/Template/NewBudget_Blank.xlsx
+++ b/src/ChurchBudgetReportGenerator/Template/NewBudget_Blank.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\ChurchBudgetReportGenerator\src\ChurchBudgetReportGenerator\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\buf\Church\Repo\ChurchBudgetReportGenerator\src\ChurchBudgetReportGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4DD6BF-7C9F-4898-B001-068AD8838D30}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9E501E-AFE2-4F8C-8A98-86BC69EB71EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="17670" windowHeight="15360" xr2:uid="{67767A2A-310A-4817-A7AA-58C3A9D342FE}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{67767A2A-310A-4817-A7AA-58C3A9D342FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="2" r:id="rId1"/>
     <sheet name="Settings" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Transactions!$A$1:$F$12</definedName>
     <definedName name="AccountType">Settings!$A$2:$A$3</definedName>
     <definedName name="Expenses">Settings!$B$3:$DA$3</definedName>
     <definedName name="Revenue">Settings!$B$2:$DA$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -190,6 +197,16 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -207,16 +224,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -231,10 +238,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BD3654E-3251-48C4-BB86-54F1AB2C1B70}" name="Funds" displayName="Funds" ref="A8:B20" totalsRowShown="0" headerRowBorderDxfId="3" headerRowCellStyle="Heading 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BD3654E-3251-48C4-BB86-54F1AB2C1B70}" name="Funds" displayName="Funds" ref="A8:B20" totalsRowShown="0" headerRowBorderDxfId="1" headerRowCellStyle="Heading 3">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6D363210-995F-48AD-B76F-76D57E9F9928}" name="Fund Types"/>
-    <tableColumn id="2" xr3:uid="{CC56FD19-18B5-4344-8A76-FA23E8765CA4}" name="Fund Beginning Amount" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{CC56FD19-18B5-4344-8A76-FA23E8765CA4}" name="Fund Beginning Amount" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -540,19 +547,19 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="3" customWidth="1"/>
+    <col min="1" max="2" width="10.41015625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.5859375" customWidth="1"/>
+    <col min="4" max="4" width="29.1171875" customWidth="1"/>
+    <col min="5" max="5" width="31.703125" customWidth="1"/>
+    <col min="6" max="6" width="18.5859375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -573,7 +580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="2">
         <v>43493</v>
       </c>
@@ -593,7 +600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>43494</v>
       </c>
@@ -613,7 +620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>43466</v>
       </c>
@@ -633,7 +640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>43497</v>
       </c>
@@ -653,7 +660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>43525</v>
       </c>
@@ -673,7 +680,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>43556</v>
       </c>
@@ -693,7 +700,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="2">
         <v>43586</v>
       </c>
@@ -713,7 +720,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
         <v>43586</v>
       </c>
@@ -733,7 +740,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="2">
         <v>43466</v>
       </c>
@@ -753,7 +760,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
         <v>43493</v>
       </c>
@@ -773,7 +780,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="2">
         <v>43466</v>
       </c>
@@ -795,10 +802,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>C1="Expenses"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>C1="Revenue"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -838,13 +845,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.41015625" customWidth="1"/>
+    <col min="2" max="2" width="22.5859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -852,7 +859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -872,7 +879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -886,7 +893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -894,7 +901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -902,7 +909,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -910,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -918,7 +925,7 @@
         <v>3400</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -926,7 +933,7 @@
         <v>187000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -934,25 +941,25 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B20" s="3"/>
     </row>
   </sheetData>

</xml_diff>